<commit_message>
Class cleanup / email functionality progress
</commit_message>
<xml_diff>
--- a/CRHT_0228100406 (1).xlsx
+++ b/CRHT_0228100406 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Desktop\WestSim_App\WestSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2803B0-1E9E-4EE1-8083-E9A1D94F8300}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2652AEEC-FF85-409C-A979-8CDC94B266D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cr_srres" sheetId="1" r:id="rId1"/>
@@ -1631,7 +1631,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1641,6 +1641,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1657,10 +1663,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2046,7 +2053,7 @@
   <dimension ref="A1:FE16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3039,7 +3046,7 @@
       <c r="A3" t="s">
         <v>185</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>186</v>
       </c>
       <c r="C3" t="s">
@@ -3051,7 +3058,7 @@
       <c r="E3" s="1">
         <v>43525</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>189</v>
       </c>
       <c r="G3" t="s">
@@ -3099,13 +3106,13 @@
       <c r="U3" t="s">
         <v>192</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="3" t="s">
         <v>195</v>
       </c>
       <c r="Y3" t="s">

</xml_diff>

<commit_message>
email cleanup / cage code dictionary revamp
</commit_message>
<xml_diff>
--- a/CRHT_0228100406 (1).xlsx
+++ b/CRHT_0228100406 (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avinash Patel\Desktop\WestSim_App\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2652AEEC-FF85-409C-A979-8CDC94B266D5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84C0DDB-3773-474B-BB10-71CF8C3BA3B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3046,7 +3046,7 @@
       <c r="A3" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>186</v>
       </c>
       <c r="C3" t="s">
@@ -3058,7 +3058,7 @@
       <c r="E3" s="1">
         <v>43525</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>189</v>
       </c>
       <c r="G3" t="s">
@@ -3067,7 +3067,7 @@
       <c r="H3" t="s">
         <v>167</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
@@ -3106,7 +3106,7 @@
       <c r="U3" t="s">
         <v>192</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V3" t="s">
         <v>193</v>
       </c>
       <c r="W3" s="3" t="s">

</xml_diff>